<commit_message>
Preparing Mission API Contract info
</commit_message>
<xml_diff>
--- a/Rumi/MissionsRewards.xlsx
+++ b/Rumi/MissionsRewards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B014088B-1ECF-4373-B83A-D4F8D9D8140E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB413BE-7E07-44ED-A2EC-728185DAC575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="3" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="2" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Raffle Mission Flow" sheetId="12" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="149">
   <si>
     <t>UI</t>
   </si>
@@ -6036,9 +6036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED923DA8-A6DE-4F8B-82AF-4BD2B1222232}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6331,9 +6331,7 @@
       <c r="C8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>93</v>
-      </c>
+      <c r="D8" s="11"/>
       <c r="E8" s="12" t="s">
         <v>60</v>
       </c>
@@ -6365,7 +6363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>95</v>
       </c>
@@ -6563,7 +6561,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6571,9 +6570,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89586828-2EC7-4376-8765-C9B5A4503640}">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7051,8 +7050,8 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7456,8 +7455,8 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Pre removal Profile Nav Button
</commit_message>
<xml_diff>
--- a/Rumi/MissionsRewards.xlsx
+++ b/Rumi/MissionsRewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB413BE-7E07-44ED-A2EC-728185DAC575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B904D5-32EB-4CA8-AF22-218A0F50F4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="2" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="150">
   <si>
     <t>UI</t>
   </si>
@@ -4135,51 +4135,6 @@
   <si>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">status= </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">'fulfilled' 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>fulfilled_at</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> set</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="11"/>
         <color theme="5"/>
         <rFont val="Aptos Narrow"/>
@@ -4701,6 +4656,76 @@
         <scheme val="minor"/>
       </rPr>
       <t>='scheduled'</t>
+    </r>
+  </si>
+  <si>
+    <t>physical_gift_redemption.tracking_number set</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">status= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">'fulfilled' 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fulfilled_at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> set
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>activation_date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> set</t>
     </r>
   </si>
 </sst>
@@ -5214,7 +5239,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6038,7 +6063,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6308,7 +6333,7 @@
         <v>87</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>47</v>
@@ -6509,7 +6534,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>20</v>
@@ -6572,7 +6597,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6842,7 +6867,7 @@
         <v>87</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>47</v>
@@ -7019,14 +7044,16 @@
       <c r="O11" s="6"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -7051,7 +7078,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9:D10"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7314,7 +7341,7 @@
         <v>87</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -7380,7 +7407,7 @@
         <v>60</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>8</v>
@@ -7415,13 +7442,13 @@
         <v>47</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>8</v>
@@ -7456,7 +7483,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7527,13 +7554,13 @@
         <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>128</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>47</v>
@@ -7648,7 +7675,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>47</v>
@@ -7719,7 +7746,7 @@
         <v>87</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -7744,7 +7771,7 @@
         <v>60</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>13</v>
@@ -7773,7 +7800,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>47</v>
@@ -7785,7 +7812,7 @@
         <v>60</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>13</v>
@@ -7814,7 +7841,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>47</v>
@@ -7826,7 +7853,7 @@
         <v>60</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
In process of developing Admin pages
</commit_message>
<xml_diff>
--- a/Rumi/MissionsRewards.xlsx
+++ b/Rumi/MissionsRewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055871B8-3E7E-4DC6-A8F5-47957582D857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B8C46-6344-49EA-91AC-19151E755A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
   </bookViews>
@@ -46,7 +46,7 @@
     <author>Jorge Naupari</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{66125775-3CF0-41B7-8ADE-E07C2550405D}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{66125775-3CF0-41B7-8ADE-E07C2550405D}">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="158">
   <si>
     <t>UI</t>
   </si>
@@ -194,51 +194,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> = Green Button to participate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TRUE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Your gift is on the way
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>FALSE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = Claim your gift!</t>
     </r>
   </si>
   <si>
@@ -4570,6 +4525,18 @@
       </rPr>
       <t>=true</t>
     </r>
+  </si>
+  <si>
+    <t>UI = CARD STATE: Dormant</t>
+  </si>
+  <si>
+    <t>UI = CARD STATE: Raffle Available</t>
+  </si>
+  <si>
+    <t>UI = CARD STATE: Raffle Processing</t>
+  </si>
+  <si>
+    <t>UI = CARD STATE: Raffle Claim</t>
   </si>
 </sst>
 </file>
@@ -5088,19 +5055,20 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="62.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="59.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="59.7109375" style="2" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="4"/>
     <col min="12" max="12" width="62.5703125" style="1" customWidth="1"/>
     <col min="13" max="14" width="14.140625" style="1" customWidth="1"/>
@@ -5111,44 +5079,44 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I1" s="3"/>
       <c r="K1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="O1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>0</v>
@@ -5156,43 +5124,41 @@
     </row>
     <row r="2" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>45</v>
+        <v>28</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>153</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>3</v>
@@ -5200,239 +5166,239 @@
     </row>
     <row r="3" spans="1:16" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="L3" s="2"/>
       <c r="M3" s="6"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>52</v>
+        <v>42</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>45</v>
+      <c r="E4" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="H4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="M4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>45</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="L5" s="2"/>
       <c r="M5" s="6"/>
       <c r="O5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>33</v>
+        <v>15</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>55</v>
+        <v>32</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>12</v>
+      <c r="G6" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>46</v>
+        <v>16</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>157</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>56</v>
+      <c r="D7" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="H7" s="11" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="H8" s="11" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
-      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="9"/>
       <c r="K10" s="8"/>
     </row>
   </sheetData>
@@ -5465,7 +5431,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -5474,155 +5440,155 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="E2" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>80</v>
-      </c>
       <c r="G6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5672,7 +5638,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -5681,347 +5647,347 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="112.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>108</v>
-      </c>
       <c r="I9" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>110</v>
-      </c>
       <c r="I10" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -6058,7 +6024,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -6067,22 +6033,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J1" s="3"/>
       <c r="L1" s="3" t="s">
@@ -6091,31 +6057,31 @@
     </row>
     <row r="2" spans="1:12" ht="112.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>119</v>
-      </c>
       <c r="F2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>3</v>
@@ -6123,247 +6089,247 @@
     </row>
     <row r="3" spans="1:12" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="I9" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="H10" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="H10" s="12" t="s">
-        <v>140</v>
-      </c>
       <c r="I10" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6422,7 +6388,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -6431,35 +6397,35 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="3"/>
       <c r="K1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="O1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>0</v>
@@ -6467,43 +6433,43 @@
     </row>
     <row r="2" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>3</v>
@@ -6511,26 +6477,26 @@
     </row>
     <row r="3" spans="1:16" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="6"/>
@@ -6538,65 +6504,65 @@
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="6"/>
@@ -6604,64 +6570,64 @@
     </row>
     <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H7" s="11"/>
       <c r="M7" s="6"/>
@@ -6670,125 +6636,125 @@
     </row>
     <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>125</v>
-      </c>
       <c r="H10" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -6826,7 +6792,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
@@ -6835,35 +6801,35 @@
         <v>1</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I1" s="3"/>
       <c r="K1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="O1" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>0</v>
@@ -6871,41 +6837,41 @@
     </row>
     <row r="2" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>127</v>
-      </c>
       <c r="F2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>3</v>
@@ -6913,26 +6879,26 @@
     </row>
     <row r="3" spans="1:16" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="6"/>
@@ -6940,65 +6906,65 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="6"/>
@@ -7006,64 +6972,64 @@
     </row>
     <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H7" s="11"/>
       <c r="M7" s="6"/>
@@ -7072,84 +7038,84 @@
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="K8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Post signup page fix
</commit_message>
<xml_diff>
--- a/Rumi/MissionsRewards.xlsx
+++ b/Rumi/MissionsRewards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103EDF9D-FDB0-4CFB-944F-0351CCCE3A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE08D995-F8A3-445E-B412-27D580EC41A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="2" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Raffle Mission Flow" sheetId="12" r:id="rId1"/>
@@ -4903,6 +4903,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3800980</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1590881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8444A81B-AE23-7C94-890E-B1AB6215DBF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13973175" y="495300"/>
+          <a:ext cx="3620005" cy="1476581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -5036,7 +5085,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -5536,9 +5585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69F2FBC-5206-4512-A557-61D9DB1505F7}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5715,7 +5764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>41</v>
       </c>
@@ -5744,7 +5793,7 @@
       <c r="M5" s="6"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -5785,7 +5834,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
@@ -5826,7 +5875,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
@@ -5904,7 +5953,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6118,9 +6168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED923DA8-A6DE-4F8B-82AF-4BD2B1222232}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6615,7 +6665,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
post \wsl$\Ubuntu\home\jorge\Loyalty\Rumi\BugFixes\RecurringScheduledRewardsGapIMPL.md fix. Post supabase local and remote missmatch headache
</commit_message>
<xml_diff>
--- a/Rumi/MissionsRewards.xlsx
+++ b/Rumi/MissionsRewards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\jorge\Loyalty\Rumi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746DF9F7-615E-4ACA-9D3F-124BF774F375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E2036F-CDAB-4B79-8F80-3A771F13CA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="6" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="5" xr2:uid="{FBBB1832-C785-4D1E-8B13-354005240D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Raffle Mission Flow" sheetId="12" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="171">
   <si>
     <t>UI</t>
   </si>
@@ -4706,13 +4706,81 @@
       </rPr>
       <t>='19:00:00' (2 PM EST)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">State
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Locked</t>
+    </r>
+  </si>
+  <si>
+    <t>No, status: 'recurring_cooldown' is computed by the service layer, not stored in any table.
+  Here's where each attribute comes from:
+  | API Field                           | Source   | Table.Column
+              |
+  |-------------------------------------|----------|-------------------------------------------------
+  ------------|
+  | status                              | Computed | missionService.computeStatus() looks at multiple
+   tables     |
+  | recurringData.frequency             | Database | rewards.redemption_frequency
+              |
+  | recurringData.cooldownUntil         | Database | mission_progress.cooldown_until ← NEW column
+  from migration |
+  | recurringData.cooldownDaysRemaining | Computed | Service layer calculates from cooldown_until
+              |
+  | recurringData.isInCooldown          | Computed | Service layer: NOW() &lt; cooldown_until
+              |
+  The 17 statuses are all computed, not stored. computeStatus() in missionService.ts checks:
+  - mission_progress.status (active/dormant/completed)
+  - redemptions.status (claimable/claimed/fulfilled/concluded/rejected)
+  - mission_progress.cooldown_until (for recurring_cooldown)
+  - commission_boost_redemptions.boost_status
+  - physical_gift_redemptions.shipped_at
+  - raffle_participations.is_winner
+  - etc.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> status: 'recurring_cooldown'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Explanation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="15"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>For Status (D)</t>
+    </r>
+  </si>
+  <si>
+    <t>Can't Participate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4800,6 +4868,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4836,7 +4920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -4882,6 +4966,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5491,16 +5584,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3276600</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1261467</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3590925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1366242</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5523,7 +5616,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16411575" y="4457700"/>
+          <a:off x="20707350" y="4200525"/>
           <a:ext cx="3105150" cy="1261467"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5535,16 +5628,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>3543771</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3858096</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1381304</xdr:rowOff>
+      <xdr:rowOff>1314629</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5567,8 +5660,145 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16411575" y="5676900"/>
+          <a:off x="20707350" y="5610225"/>
           <a:ext cx="3372321" cy="1286054"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3667590</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1152643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F2BCE0D-61C7-AA75-BE3D-D8814A7DCB6C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16573500" y="5886450"/>
+          <a:ext cx="3334215" cy="847843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>571500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2333625</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1091209</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29C2F65C-24BB-48C2-90F9-0FFC0D248C3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16325850" y="4667250"/>
+          <a:ext cx="2247900" cy="519709"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2248552</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>942975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF2D2B8A-EB13-4697-F6F6-67E192219725}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7381875" y="5181600"/>
+          <a:ext cx="2124727" cy="876300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7633,11 +7863,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFE6C49-2D15-4931-B74C-66714C458773}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7650,11 +7880,11 @@
     <col min="6" max="6" width="30" style="1" customWidth="1"/>
     <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="59.7109375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="4"/>
+    <col min="9" max="12" width="59.7109375" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
@@ -7680,8 +7910,11 @@
         <v>6</v>
       </c>
       <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="112.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
@@ -7705,7 +7938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="105" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>47</v>
       </c>
@@ -7729,7 +7962,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>42</v>
       </c>
@@ -7753,7 +7986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>41</v>
       </c>
@@ -7777,7 +8010,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -7801,7 +8034,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="117" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
@@ -7825,7 +8058,7 @@
       </c>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:9" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
@@ -7851,7 +8084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
@@ -7886,14 +8119,82 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DA44F0-C73B-4A87-B179-4A021F5522AA}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="61.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="18"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="18"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="75.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="18"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="18"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
+    </row>
+    <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>